<commit_message>
Update the SG model
# Project Update: File Organization and Model Enhancements

### Summary of Changes

1. **File Restructuring**:
   - Rearranged the project files to improve organization and code clarity.

2. **DFIG Files Removal**:
   - Deleted all files related to the Doubly-Fed Induction Generator (DFIG) models to focus the repository on core synchronous generator components.

3. **Synchronous Generator (SG) Updates**:
   - Enhanced and separated the SG-related files, refining the SG models and updating dependencies.
   - Modularized SG code to improve reusability and future development.
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/IEEE_14BusFullOrder/IEEE_14BusFullOrder.xlsx
+++ b/Examples/AcPowerSystem/IEEE_14BusFullOrder/IEEE_14BusFullOrder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11655" activeTab="1"/>
+    <workbookView windowWidth="16200" windowHeight="24855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1793,8 +1793,8 @@
   <sheetPr/>
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -1839,19 +1839,19 @@
         <v>30</v>
       </c>
       <c r="C3" s="6">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="D3" s="6">
         <v>0.5</v>
       </c>
       <c r="E3" s="6">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H3" s="6">
         <v>0.45</v>
@@ -1863,7 +1863,7 @@
         <v>0.02</v>
       </c>
       <c r="K3" s="6">
-        <v>9</v>
+        <v>9.32</v>
       </c>
       <c r="L3" s="6">
         <v>0.05</v>
@@ -1934,7 +1934,7 @@
         <v>0.02</v>
       </c>
       <c r="K4" s="6">
-        <v>9</v>
+        <v>8.57</v>
       </c>
       <c r="L4" s="6">
         <v>0.05</v>
@@ -1981,19 +1981,19 @@
         <v>30</v>
       </c>
       <c r="C5" s="6">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="D5" s="6">
         <v>0.5</v>
       </c>
       <c r="E5" s="6">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H5" s="6">
         <v>0.45</v>
@@ -2005,7 +2005,7 @@
         <v>0.02</v>
       </c>
       <c r="K5" s="6">
-        <v>9</v>
+        <v>8.88</v>
       </c>
       <c r="L5" s="6">
         <v>0.05</v>
@@ -2076,7 +2076,7 @@
         <v>0.02</v>
       </c>
       <c r="K6" s="6">
-        <v>9</v>
+        <v>8.32</v>
       </c>
       <c r="L6" s="6">
         <v>0.05</v>
@@ -2147,7 +2147,7 @@
         <v>0.02</v>
       </c>
       <c r="K7" s="6">
-        <v>9</v>
+        <v>9.21</v>
       </c>
       <c r="L7" s="6">
         <v>0.05</v>

</xml_diff>